<commit_message>
created convolution method in utility that takes the average of non-zero values in 3x3 blocks, also updated excel files to fix files that we overlooked in my pmax program
</commit_message>
<xml_diff>
--- a/Pmax/Old Pmax/Sample 2/Unnormalized_Pmax_Sample_2A_100kHz.xlsx
+++ b/Pmax/Old Pmax/Sample 2/Unnormalized_Pmax_Sample_2A_100kHz.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,933 +436,633 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>File Name</t>
+          <t>Loc</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnormalized P_max</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Electrode Locations</t>
+          <t>P_max</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A1_bipolar_20V_100kHz.txt</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>50.839116</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A3_bipolar_20V_100kHz.txt</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>55.73607</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>A3</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A7_bipolar_20V_100kHz.txt</t>
+          <t>A7</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>59.549868</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>A7</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A11_bipolar_20V_100kHz.txt</t>
+          <t>A11</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>58.990997</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>A11</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A13_bipolar_20V_100kHz.txt</t>
+          <t>A13</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>52.903483</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>A13</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>A15_bipolar_20V_100kHz.txt</t>
+          <t>A15</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>58.164522</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>A15</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>B5_bipolar_20V_100kHz.txt</t>
+          <t>B5</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>70.60351199999999</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>B5</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>B10_bipolar_20V_100kHz.txt</t>
+          <t>B10</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>72.37661</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>B10</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C1_bipolar_20V_100kHz.txt</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>43.2989</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C5_bipolar_20V_100kHz.txt</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>81.75727999999999</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>C5</t>
-        </is>
+        <v>78.67165300000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C7_bipolar_20V_100kHz.txt</t>
+          <t>C5</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>78.7026</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>C7</t>
-        </is>
+        <v>81.75727999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C9_bipolar_20V_100kHz.txt</t>
+          <t>C7</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>78.74082900000001</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>C9</t>
-        </is>
+        <v>78.7026</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C11_bipolar_20V_100kHz.txt</t>
+          <t>C9</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>84.25308800000001</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>C11</t>
-        </is>
+        <v>78.74082900000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C13_bipolar_20V_100kHz.txt</t>
+          <t>C11</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>89.883674</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>C13</t>
-        </is>
+        <v>84.25308800000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C15_bipolar_20V_100kHz.txt</t>
+          <t>C13</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>98.033734</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>C15</t>
-        </is>
+        <v>89.883674</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>D8_bipolar_20V_100kHz.txt</t>
+          <t>C15</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>86.643311</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>D8</t>
-        </is>
+        <v>98.033734</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>D10_bipolar_20V_100kHz.txt</t>
+          <t>D8</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>94.267267</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>D10</t>
-        </is>
+        <v>86.643311</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>E1_bipolar_20V_100kHz.txt</t>
+          <t>D10</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>27.439324</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>E1</t>
-        </is>
+        <v>94.267267</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>E3_bipolar_20V_100kHz.txt</t>
+          <t>E1</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>93.415306</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
+        <v>27.439324</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>E5_bipolar_20V_100kHz.txt</t>
+          <t>E3</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>94.751501</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>E5</t>
-        </is>
+        <v>93.415306</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>E11_bipolar_20V_100kHz.txt</t>
+          <t>E5</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>96.801304</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>E11</t>
-        </is>
+        <v>94.751501</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>E13_bipolar_20V_100kHz.txt</t>
+          <t>E11</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>89.58148300000001</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>E13</t>
-        </is>
+        <v>96.801304</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>E15_bipolar_20V_100kHz.txt</t>
+          <t>E13</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>119.869778</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>E15</t>
-        </is>
+        <v>89.58148300000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>F5_bipolar_20V_100kHz.txt</t>
+          <t>E15</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>99.819575</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>F5</t>
-        </is>
+        <v>119.869778</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>F7_bipolar_20V_100kHz.txt</t>
+          <t>F5</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>101.918529</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>F7</t>
-        </is>
+        <v>99.819575</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>F9_bipolar_20V_100kHz.txt</t>
+          <t>F7</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>105.351858</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
+        <v>101.918529</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>G1_bipolar_20V_100kHz.txt</t>
+          <t>F9</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>22.32938</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>G1</t>
-        </is>
+        <v>105.351858</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>G3_bipolar_20V_100kHz.txt</t>
+          <t>G1</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>106.263893</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
+        <v>22.32938</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>G7_bipolar_20V_100kHz.txt</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>108.362848</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>G7</t>
-        </is>
+        <v>106.263893</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>G11_bipolar_20V_100kHz.txt</t>
+          <t>G7</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>115.975881</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>G11</t>
-        </is>
+        <v>108.362848</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>G12_bipolar_20V_100kHz.txt</t>
+          <t>G11</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>111.723359</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>G12</t>
-        </is>
+        <v>115.975881</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>G15_bipolar_20V_100kHz.txt</t>
+          <t>G12</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>122.161698</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>G15</t>
-        </is>
+        <v>111.723359</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>H6_bipolar_20V_100kHz.txt</t>
+          <t>G15</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>112.484299</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>H6</t>
-        </is>
+        <v>122.161698</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>H9_bipolar_20V_100kHz.txt</t>
+          <t>H6</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>114.452182</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>H9</t>
-        </is>
+        <v>112.484299</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>I3_bipolar_20V_100kHz.txt</t>
+          <t>H9</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>114.06261</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>I3</t>
-        </is>
+        <v>114.452182</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>I5_bipolar_20V_100kHz.txt</t>
+          <t>I3</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>113.55107</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>I5</t>
-        </is>
+        <v>114.06261</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>I8_bipolar_20V_100kHz.txt</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>111.919966</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>I8</t>
-        </is>
+        <v>113.55107</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>I12_bipolar_20V_100kHz.txt</t>
+          <t>I8</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>121.732077</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>I12</t>
-        </is>
+        <v>111.919966</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>I15_bipolar_20V_100kHz.txt</t>
+          <t>I12</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>133.646784</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>I15</t>
-        </is>
+        <v>121.732077</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>J1_bipolar_20V_100kHz.txt</t>
+          <t>I15</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>21.94709</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>J1</t>
-        </is>
+        <v>133.646784</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>J10_bipolar_20V_100kHz.txt</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>111.754307</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>J10</t>
-        </is>
+        <v>21.94709</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>K1_bipolar_20V_100kHz.txt</t>
+          <t>J10</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>31.061977</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>K1</t>
-        </is>
+        <v>111.754307</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>K6_bipolar_20V_100kHz.txt</t>
+          <t>K1</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>108.557634</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>K6</t>
-        </is>
+        <v>31.061977</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>K8_bipolar_20V_100kHz.txt</t>
+          <t>K6</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>103.114551</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>K8</t>
-        </is>
+        <v>108.557634</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>K10_bipolar_20V_100kHz.txt</t>
+          <t>K8</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>111.195435</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>K10</t>
-        </is>
+        <v>103.114551</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>K12_bipolar_20V_100kHz.txt</t>
+          <t>K10</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>113.583838</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>K12</t>
-        </is>
+        <v>111.195435</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>L3_bipolar_20V_100kHz.txt</t>
+          <t>K12</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>105.246273</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>L3</t>
-        </is>
+        <v>113.583838</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>L9_bipolar_20V_100kHz.txt</t>
+          <t>L3</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>117.747158</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>L9</t>
-        </is>
+        <v>105.246273</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>M1_bipolar_20V_100kHz.txt</t>
+          <t>L9</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>33.736187</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>M1</t>
-        </is>
+        <v>117.747158</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>M3_bipolar_20V_100kHz.txt</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>103.504123</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>M3</t>
-        </is>
+        <v>33.736187</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>M5_bipolar_20V_100kHz.txt</t>
+          <t>M3</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>105.180738</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>M5</t>
-        </is>
+        <v>103.504123</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>M7_bipolar_20V_100kHz.txt</t>
+          <t>M5</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>100.7753</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>M7</t>
-        </is>
+        <v>105.180738</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>M10_bipolar_20V_100kHz.txt</t>
+          <t>M7</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>108.703268</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>M10</t>
-        </is>
+        <v>100.7753</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>M12_bipolar_20V_100kHz.txt</t>
+          <t>M10</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>116.265329</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>M12</t>
-        </is>
+        <v>108.703268</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>N14_bipolar_20V_100kHz.txt</t>
+          <t>M12</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>121.863148</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>N14</t>
-        </is>
+        <v>116.265329</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>O1_bipolar_20V_100kHz.txt</t>
+          <t>N14</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>42.880202</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>O1</t>
-        </is>
+        <v>121.863148</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>O3_bipolar_20V_100kHz.txt</t>
+          <t>O1</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>79.14678499999999</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>O3</t>
-        </is>
+        <v>42.880202</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>O6_bipolar_20V_100kHz.txt</t>
+          <t>O3</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>96.26427700000001</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>O6</t>
-        </is>
+        <v>79.14678499999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>O8_bipolar_20V_100kHz.txt</t>
+          <t>O6</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>90.171302</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>O8</t>
-        </is>
+        <v>96.26427700000001</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>O10_bipolar_20V_100kHz.txt</t>
+          <t>O8</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>93.808519</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>O10</t>
-        </is>
+        <v>90.171302</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>O12_bipolar_20V_100kHz.txt</t>
+          <t>O10</t>
         </is>
       </c>
       <c r="B62" t="n">
+        <v>93.808519</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>O12</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
         <v>95.798248</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>O12</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>